<commit_message>
Working on Truing Model
eta_optical is good.  The convection between the receiver and amb had a
delta t of >50. Using the cca temps on module 2&3. the conv, and cond
loss at the receiver are now in ~range.  Balancing has mainly been
looking at the 3 temps on s3m3 and s3m2.  Still need to true heat loss
between runs
</commit_message>
<xml_diff>
--- a/True Up WorkFlow.xlsx
+++ b/True Up WorkFlow.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Truing Up Parameter on Modelcia In studio </t>
   </si>
@@ -66,13 +66,61 @@
   </si>
   <si>
     <t>Start at module s3m6. Look at temperature increase over cell</t>
+  </si>
+  <si>
+    <t>Little high, will attempt to adjust the theta / heat loss</t>
+  </si>
+  <si>
+    <t>STEP 2. Checking the temps at the modules. Module 6 show below. WaterBlock resivitiy at 1.6</t>
+  </si>
+  <si>
+    <t>Realize that we have the we can use the reciver water block reporting from the experiment.  Now showing too much heat going to point, aka the CCA resitance needs to go up</t>
+  </si>
+  <si>
+    <t>CLOSER</t>
+  </si>
+  <si>
+    <t>Real Resistivity_Cell = 4</t>
+  </si>
+  <si>
+    <t>Real Resistivity_Cell = 0.2</t>
+  </si>
+  <si>
+    <t>spec sheet says</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Cond_RecToEnv = 5</t>
+  </si>
+  <si>
+    <t>Cond_RecToEnv =10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change to </t>
+  </si>
+  <si>
+    <t>Conv at 0.5</t>
+  </si>
+  <si>
+    <t>THAT’S BETTER</t>
+  </si>
+  <si>
+    <t>restitbty from 1.6 to 1.4</t>
+  </si>
+  <si>
+    <t>Too get above I used the following parameters</t>
+  </si>
+  <si>
+    <t>WaterPlate Resistivity to 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +138,14 @@
     <font>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -116,11 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -284,6 +341,386 @@
         <a:xfrm>
           <a:off x="0" y="12763500"/>
           <a:ext cx="4656771" cy="3295650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>398933</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>27714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="17135475"/>
+          <a:ext cx="8933333" cy="6885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>284267</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>75351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="24517350"/>
+          <a:ext cx="11866667" cy="6790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>493790</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>122952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="31994475"/>
+          <a:ext cx="12076190" cy="6980952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>247169</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>28029</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12249150" y="24412575"/>
+          <a:ext cx="3847619" cy="4371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>83962</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>103881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="39614475"/>
+          <a:ext cx="14104762" cy="7152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>512838</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>65786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="47424975"/>
+          <a:ext cx="12095238" cy="7114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>541409</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>189619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="55044975"/>
+          <a:ext cx="12123809" cy="7047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>328</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>227047</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>37190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="62664975"/>
+          <a:ext cx="12419047" cy="7276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>484269</xdr:colOff>
+      <xdr:row>403</xdr:row>
+      <xdr:rowOff>132508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="70351650"/>
+          <a:ext cx="12047619" cy="6733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>407</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>83962</xdr:colOff>
+      <xdr:row>417</xdr:row>
+      <xdr:rowOff>9287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="77724000"/>
+          <a:ext cx="14104762" cy="1904762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -558,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:U405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A326" sqref="A326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +1084,74 @@
         <v>9</v>
       </c>
     </row>
+    <row r="88" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>16</v>
+      </c>
+      <c r="R127" t="s">
+        <v>19</v>
+      </c>
+      <c r="U127" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>17</v>
+      </c>
+      <c r="B166" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>21</v>
+      </c>
+      <c r="B207" t="s">
+        <v>23</v>
+      </c>
+      <c r="E207" t="s">
+        <v>24</v>
+      </c>
+      <c r="F207" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Steps towards truing Model
</commit_message>
<xml_diff>
--- a/True Up WorkFlow.xlsx
+++ b/True Up WorkFlow.xlsx
@@ -6355,8 +6355,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Y219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE1:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
UQ for eGen and T_HTF_out
Add Upper and Lower Limits for UQ. Also, adjusted the DNI in order to
look at transient response to begin tuning the Heat capacitor of the
module receiver. For Mar 23, the data begins too late to fully analyze
the transient behavior.
</commit_message>
<xml_diff>
--- a/True Up WorkFlow.xlsx
+++ b/True Up WorkFlow.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenton\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenton\Documents\GitHub\RPI_CASE_ICS_Modelica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DAY 1 (5.3.15)" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Day 3 (5.22.15)" sheetId="4" r:id="rId4"/>
     <sheet name="From Day 3 step  0" sheetId="5" r:id="rId5"/>
     <sheet name="Day 4 (5.23.15)" sheetId="6" r:id="rId6"/>
+    <sheet name="Day 5 (5.24.15)" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t xml:space="preserve">Truing Up Parameter on Modelcia In studio </t>
   </si>
@@ -309,6 +310,18 @@
   <si>
     <t>when view the transient fit, the temp from modelica match very nicley</t>
   </si>
+  <si>
+    <t>Adding Uncertainty in Measured data to ICSolar.mo</t>
+  </si>
+  <si>
+    <t>1. Adding measured Egen_Uncertainity</t>
+  </si>
+  <si>
+    <t>2. Adding Uncertaintiy to T_HTF_Out</t>
+  </si>
+  <si>
+    <t>3. Tuning the Heat capacitor at the module to have the proper transient response</t>
+  </si>
 </sst>
 </file>
 
@@ -559,11 +572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346205968"/>
-        <c:axId val="346207144"/>
+        <c:axId val="611263824"/>
+        <c:axId val="611264216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346205968"/>
+        <c:axId val="611263824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,12 +633,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346207144"/>
+        <c:crossAx val="611264216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346207144"/>
+        <c:axId val="611264216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,7 +695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346205968"/>
+        <c:crossAx val="611263824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2629,6 +2642,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>93714</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>56119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="12285714" cy="8247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>17524</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>75167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9525000"/>
+          <a:ext cx="12209524" cy="8266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -15726,7 +15820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
@@ -15959,4 +16053,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Draft of Modelica Scripting
Attempt at automating the true up process. Brute force at the moment;
simulate multiple trials then bring to excel to observe the quadractic
best fit to find -b/2a
</commit_message>
<xml_diff>
--- a/True Up WorkFlow.xlsx
+++ b/True Up WorkFlow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DAY 1 (5.3.15)" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,11 @@
     <sheet name="RMSE From Day2" sheetId="3" r:id="rId3"/>
     <sheet name="Day 3 (5.22.15)" sheetId="4" r:id="rId4"/>
     <sheet name="From Day 3 step  0" sheetId="5" r:id="rId5"/>
-    <sheet name="Day 4 (5.23.15)" sheetId="6" r:id="rId6"/>
-    <sheet name="Day 5 (5.24.15)" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
+    <sheet name="Day 4 (5.23.15)" sheetId="6" r:id="rId7"/>
+    <sheet name="Day 5 (5.24.15)" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -327,10 +328,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +386,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -407,7 +415,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -425,6 +433,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -445,6 +455,357 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0610061575002744E-2"/>
+                  <c:y val="-0.72373396033829107"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>63.563209289468602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.986053650066101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1890990896620099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7160336563324199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="617785880"/>
+        <c:axId val="365785208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="617785880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365785208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="365785208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="617785880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -572,11 +933,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="611263824"/>
-        <c:axId val="611264216"/>
+        <c:axId val="365787168"/>
+        <c:axId val="365783640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="611263824"/>
+        <c:axId val="365787168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,12 +994,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="611264216"/>
+        <c:crossAx val="365783640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="611264216"/>
+        <c:axId val="365783640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +1056,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="611263824"/>
+        <c:crossAx val="365787168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -784,7 +1145,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2533,6 +3450,41 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2642,7 +3594,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -15818,6 +16770,71 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.45</v>
+      </c>
+      <c r="B1">
+        <v>0.5</v>
+      </c>
+      <c r="C1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>63.563209289468602</v>
+      </c>
+      <c r="B2">
+        <v>20.986053650066101</v>
+      </c>
+      <c r="C2">
+        <v>2.1890990896620099</v>
+      </c>
+      <c r="D2">
+        <v>6.7160336563324199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5324.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>4710.4</f>
+        <v>4710.3999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <f>A4/(A5*2)</f>
+        <v>0.56519616168478271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
@@ -16055,12 +17072,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>